<commit_message>
New level Trap doors Death by spike traps
</commit_message>
<xml_diff>
--- a/darkworld/model/data/floor builder Intro Worlds.xlsx
+++ b/darkworld/model/data/floor builder Intro Worlds.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\DarkWorld\darkworld\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C5FE9A-14BA-4477-9CE6-03B4D83A2805}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F820D3-5929-4FCD-B7F2-B8E4240B3B70}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16515" yWindow="2220" windowWidth="25065" windowHeight="15840" tabRatio="904" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="904" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="49" r:id="rId1"/>
@@ -6686,22 +6686,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="3" priority="4">
+    <cfRule type="expression" dxfId="41" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="2" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="39" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7415,7 +7415,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="12" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="F10" s="12" t="s">
         <v>4</v>
@@ -7469,11 +7469,11 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v>#      #    #   n  #</v>
+        <v>#   A  #    #   n  #</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>'#      #    #   n  #',</v>
+        <v>'#   A  #    #   n  #',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -8429,22 +8429,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="41" priority="4">
+    <cfRule type="expression" dxfId="37" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="40" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="39" priority="2">
+    <cfRule type="expression" dxfId="35" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="38" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10172,22 +10172,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="37" priority="4">
+    <cfRule type="expression" dxfId="33" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="36" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="35" priority="2">
+    <cfRule type="expression" dxfId="31" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="34" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10200,7 +10200,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2971BDDA-8A19-4180-8C39-872748330347}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
@@ -10922,7 +10922,7 @@
         <v>4</v>
       </c>
       <c r="L10" s="12" t="s">
-        <v>4</v>
+        <v>78</v>
       </c>
       <c r="M10" s="12" t="s">
         <v>4</v>
@@ -10955,11 +10955,11 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v>#     B#       D   #</v>
+        <v>#     B#   z   D   #</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>'#     B#       D   #',</v>
+        <v>'#     B#   z   D   #',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -11006,7 +11006,7 @@
         <v>4</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>78</v>
+        <v>4</v>
       </c>
       <c r="P11" s="12" t="s">
         <v>26</v>
@@ -11030,11 +11030,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v>#     B#      z##E##</v>
+        <v>#     B#       ##E##</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'#     B#      z##E##',</v>
+        <v>'#     B#       ##E##',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -11915,22 +11915,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="33" priority="4">
+    <cfRule type="expression" dxfId="29" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="32" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="31" priority="2">
+    <cfRule type="expression" dxfId="27" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="30" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13658,22 +13658,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A21:Y25 U1:Y20">
-    <cfRule type="expression" dxfId="29" priority="4">
+    <cfRule type="expression" dxfId="25" priority="4">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21:Z25 U1:Z20">
-    <cfRule type="cellIs" dxfId="28" priority="3" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="3" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="expression" dxfId="27" priority="2">
+    <cfRule type="expression" dxfId="23" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:T20">
-    <cfRule type="cellIs" dxfId="26" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13687,7 +13687,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14231,7 +14231,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="D8" s="12" t="s">
         <v>26</v>
@@ -14291,11 +14291,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">#  #                </v>
+        <v xml:space="preserve"># G#                </v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'#  #                ',</v>
+        <v>'# G#                ',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -15401,12 +15401,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="25" priority="2">
+    <cfRule type="expression" dxfId="21" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="24" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -17134,12 +17134,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="23" priority="2">
+    <cfRule type="expression" dxfId="19" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="22" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18867,12 +18867,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="21" priority="2">
+    <cfRule type="expression" dxfId="17" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="20" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20600,12 +20600,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="19" priority="2">
+    <cfRule type="expression" dxfId="15" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="18" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20618,7 +20618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A466A983-0CC0-4A22-B25B-02607ECF604A}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
@@ -21091,7 +21091,7 @@
         <v>4</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>4</v>
+        <v>60</v>
       </c>
       <c r="E7" s="12" t="s">
         <v>4</v>
@@ -21148,11 +21148,11 @@
       <c r="Y7" s="7"/>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v>#b   qB#B   ###q  b#</v>
+        <v>#b R qB#B   ###q  b#</v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'#b   qB#B   ###q  b#',</v>
+        <v>'#b R qB#B   ###q  b#',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -21160,7 +21160,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>4</v>
+        <v>47</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>4</v>
@@ -21223,11 +21223,11 @@
       <c r="Y8" s="7"/>
       <c r="AA8" t="str">
         <f t="shared" si="0"/>
-        <v>#      S    ###    #</v>
+        <v>#a     S    ###    #</v>
       </c>
       <c r="AB8" t="str">
         <f t="shared" si="1"/>
-        <v>'#      S    ###    #',</v>
+        <v>'#a     S    ###    #',</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
@@ -21385,7 +21385,7 @@
         <v>26</v>
       </c>
       <c r="B11" s="12" t="s">
-        <v>4</v>
+        <v>58</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>4</v>
@@ -21448,11 +21448,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v>#                  #</v>
+        <v>#G                 #</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  #',</v>
+        <v>'#G                 #',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -21535,7 +21535,7 @@
         <v>26</v>
       </c>
       <c r="B13" s="12" t="s">
-        <v>4</v>
+        <v>49</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>4</v>
@@ -21598,11 +21598,11 @@
       <c r="Y13" s="7"/>
       <c r="AA13" t="str">
         <f t="shared" si="0"/>
-        <v>#      S    ###    #</v>
+        <v>#h     S    ###    #</v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="1"/>
-        <v>'#      S    ###    #',</v>
+        <v>'#h     S    ###    #',</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -21622,7 +21622,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>4</v>
+        <v>57</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>44</v>
@@ -21640,7 +21640,7 @@
         <v>4</v>
       </c>
       <c r="L14" s="12" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="M14" s="12" t="s">
         <v>26</v>
@@ -21673,11 +21673,11 @@
       <c r="Y14" s="7"/>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v>#bQ   B#B  Q###   b#</v>
+        <v>#bQ  gB#B  q###   b#</v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'#bQ   B#B  Q###   b#',</v>
+        <v>'#bQ  gB#B  q###   b#',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -24076,12 +24076,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="17" priority="2">
+    <cfRule type="expression" dxfId="13" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="16" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25812,12 +25812,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="15" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="14" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -27548,12 +27548,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="13" priority="2">
+    <cfRule type="expression" dxfId="9" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="12" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29284,12 +29284,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31017,12 +31017,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="5" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="8" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -32753,12 +32753,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="7" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="6" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -35186,12 +35186,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A1:Y25">
-    <cfRule type="expression" dxfId="5" priority="2">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>AND(COLUMN()&lt;=$B$26,ROW()&lt;=$B$27)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:Z25">
-    <cfRule type="cellIs" dxfId="4" priority="1" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" stopIfTrue="1" operator="equal">
       <formula>":"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>